<commit_message>
Finished rough draft of research report and began revisions.
</commit_message>
<xml_diff>
--- a/Documentation/Test Results/Final Results.xlsx
+++ b/Documentation/Test Results/Final Results.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>Font</t>
   </si>
@@ -61,6 +60,27 @@
   </si>
   <si>
     <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Segmentation Algo</t>
+  </si>
+  <si>
+    <t># Wrong</t>
+  </si>
+  <si>
+    <t>*** out of 415 characters</t>
+  </si>
+  <si>
+    <t>Topological</t>
+  </si>
+  <si>
+    <t>X-Y Cut</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>*** Out of 174 characters</t>
   </si>
 </sst>
 </file>
@@ -379,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,6 +602,9 @@
       <c r="D15" s="1">
         <v>0.94830000000000003</v>
       </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -623,6 +646,42 @@
       </c>
       <c r="D18" s="1">
         <v>0.81399999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.8899999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>